<commit_message>
clases para el tag de movimientos contables dinamico
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataCertSaldos.xlsx
+++ b/src/test/resources/Data/AutomationDataCertSaldos.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C88BAA-94FE-4D99-BE7A-6B964E3F62E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC149F4-57C6-419B-B4EB-37387E953361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Retanqueo" sheetId="10" r:id="rId1"/>
+    <sheet name="CertificacionSaldo" sheetId="10" r:id="rId1"/>
+    <sheet name="OrigincacionPrueba" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>NumRadicado</t>
   </si>
@@ -57,19 +58,52 @@
     <t>RutaDocumento</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Prepago</t>
   </si>
   <si>
     <t>"src/test/resources/Data/CertificacionSaldos/"</t>
   </si>
   <si>
-    <t>33774</t>
-  </si>
-  <si>
-    <t>35490956</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>AccountingSource</t>
+  </si>
+  <si>
+    <t>"'ACRED','EGRESO'"</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>AcountingName</t>
+  </si>
+  <si>
+    <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
+  </si>
+  <si>
+    <t>14966328</t>
+  </si>
+  <si>
+    <t>66994</t>
+  </si>
+  <si>
+    <t>16343742</t>
+  </si>
+  <si>
+    <t>"'CSALD'"</t>
+  </si>
+  <si>
+    <t>"upper('Recaudo certificado de saldo')"</t>
+  </si>
+  <si>
+    <t>10/11/2021</t>
+  </si>
+  <si>
+    <t>FechaRegistro</t>
+  </si>
+  <si>
+    <t>27/10/2021</t>
   </si>
 </sst>
 </file>
@@ -111,11 +145,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,18 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,36 +467,131 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>18000</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>18000</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2" numberStoredAsText="1"/>
-  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A997E1-CA9F-4597-8B47-FEFC92082131}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>18000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajuste Feature y Archivos para validacion de dinamicas
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataCertSaldos.xlsx
+++ b/src/test/resources/Data/AutomationDataCertSaldos.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThainerPerez\Repositorios\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC149F4-57C6-419B-B4EB-37387E953361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBCAAE4-1C02-49A5-B2F6-B385847A4ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CertificacionSaldo" sheetId="10" r:id="rId1"/>
-    <sheet name="OrigincacionPrueba" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>NumRadicado</t>
   </si>
@@ -70,21 +69,9 @@
     <t>AccountingSource</t>
   </si>
   <si>
-    <t>"'ACRED','EGRESO'"</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>AcountingName</t>
   </si>
   <si>
-    <t>"upper('Desembolso egreso'), upper('Desembolso activación de crédito')"</t>
-  </si>
-  <si>
-    <t>14966328</t>
-  </si>
-  <si>
     <t>66994</t>
   </si>
   <si>
@@ -101,9 +88,6 @@
   </si>
   <si>
     <t>FechaRegistro</t>
-  </si>
-  <si>
-    <t>27/10/2021</t>
   </si>
 </sst>
 </file>
@@ -125,12 +109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,13 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,18 +458,18 @@
         <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -500,13 +487,13 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -514,84 +501,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A997E1-CA9F-4597-8B47-FEFC92082131}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>18000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se procede a crear el nuevo Tag de validacion dinamica para Prepagos; “@ValidarDinamicasContablesPREPAG“; En el cual se implementan los pasos necesarios para la validación haciendo uso de las nuevas variables; ”AccountingSourcePrepago” ”AccountingNamePrepago”
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/AutomationDataCertSaldos.xlsx
+++ b/src/test/resources/Data/AutomationDataCertSaldos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recursos\testautomationpom\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\ana.desarrollo59\Documents\testautomationpom\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C28984-526F-4DAB-8C25-90065B9C3EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B736B802-361B-4B24-B129-14DA454000F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="1830" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CertificacionSaldo" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>NumRadicado</t>
   </si>
@@ -69,12 +69,6 @@
     <t>AcountingName</t>
   </si>
   <si>
-    <t>66994</t>
-  </si>
-  <si>
-    <t>16343742</t>
-  </si>
-  <si>
     <t>"'CSALD'"</t>
   </si>
   <si>
@@ -84,10 +78,28 @@
     <t>FechaRegistro</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>21/12/2021</t>
+    <t>AccountingSourcePrepag</t>
+  </si>
+  <si>
+    <t>AcountingNamePrepag</t>
+  </si>
+  <si>
+    <t>"upper('Recaudo prepago')"</t>
+  </si>
+  <si>
+    <t>77513</t>
+  </si>
+  <si>
+    <t>8757940</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>14/01/2022</t>
+  </si>
+  <si>
+    <t>"'PREPAG'"</t>
   </si>
 </sst>
 </file>
@@ -419,20 +431,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894C6080-F6C9-4628-AA63-104D0AFEE608}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,18 +477,24 @@
         <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -487,13 +509,19 @@
         <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>